<commit_message>
update source files for this branch
</commit_message>
<xml_diff>
--- a/in/gaza_food_data.xlsx
+++ b/in/gaza_food_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phsrfche\Desktop\gaza_nutrition_paper\caloric_availability\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1A39A5-BD53-41FB-B8BA-612D74264FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DE4432-5755-4D98-A398-3FBC32BC35D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2128,7 +2128,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3647,7 +3647,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>